<commit_message>
takes a list of websites and automates
</commit_message>
<xml_diff>
--- a/TodoListForHeader.xlsx
+++ b/TodoListForHeader.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephlee/Desktop/puppeteer-teleos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephlee/Projects/puppeteer-teleos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB8ACB4C-12DE-9449-8885-5E388DAF7324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC39EA1B-025C-924B-95E0-7B2140140986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="23380" activeTab="2" xr2:uid="{BB39E0D0-C88E-0046-95F3-1766E0C30F43}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26540" activeTab="3" xr2:uid="{BB39E0D0-C88E-0046-95F3-1766E0C30F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="643">
   <si>
     <t>Live 04/11/21</t>
   </si>
@@ -1845,12 +1846,6 @@
     <t>greenhillvillas.com</t>
   </si>
   <si>
-    <t>(409) 787-5300</t>
-  </si>
-  <si>
-    <t>hillsidenursing.com</t>
-  </si>
-  <si>
     <t>903-396-3211</t>
   </si>
   <si>
@@ -1953,9 +1948,6 @@
     <t>903-395-2125</t>
   </si>
   <si>
-    <t>409-787-5300</t>
-  </si>
-  <si>
     <t>817-237-7231</t>
   </si>
   <si>
@@ -1972,16 +1964,20 @@
   </si>
   <si>
     <t>weird</t>
+  </si>
+  <si>
+    <t>FivePointsDeSoto.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;'&quot;@&quot;'&quot;\,"/>
+    <numFmt numFmtId="170" formatCode="\'@\'\,"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2057,8 +2053,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2068,6 +2071,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2085,7 +2094,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2115,6 +2124,22 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2432,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E1A0D0-F489-8844-90F5-42BAD6EBE1F3}">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8702,10 +8727,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB1A729-474B-F044-A3E8-D26ED482CA89}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8714,6 +8739,7 @@
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -8724,7 +8750,7 @@
         <v>577</v>
       </c>
       <c r="D1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -8742,10 +8768,10 @@
         <v>node teleosHeader  amarilloskilledcenter.com 806-352-8800</v>
       </c>
       <c r="G2" t="s">
-        <v>642</v>
-      </c>
-      <c r="H2" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -8759,14 +8785,14 @@
         <v>578</v>
       </c>
       <c r="F3" s="20" t="str">
-        <f t="shared" ref="F3:F66" si="0">"node teleosHeader  "&amp;B3&amp;" "&amp;D3</f>
+        <f t="shared" ref="F3:F65" si="0">"node teleosHeader  "&amp;B3&amp;" "&amp;D3</f>
         <v>node teleosHeader  beaumontnursingandrehab.com 409-842-3120</v>
       </c>
       <c r="G3" t="s">
-        <v>642</v>
-      </c>
-      <c r="H3" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -8784,10 +8810,10 @@
         <v>node teleosHeader  bertramnursing.com 512-355-2116</v>
       </c>
       <c r="G4" t="s">
-        <v>642</v>
-      </c>
-      <c r="H4" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -8805,10 +8831,10 @@
         <v>node teleosHeader  bigspringcenterforskilledcare.com 432-606-5012</v>
       </c>
       <c r="G5" t="s">
-        <v>642</v>
-      </c>
-      <c r="H5" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -8819,17 +8845,17 @@
         <v>581</v>
       </c>
       <c r="D6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>node teleosHeader  birchwoodnursing.com 903-395-2125</v>
       </c>
       <c r="G6" t="s">
-        <v>642</v>
-      </c>
-      <c r="H6" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -8847,10 +8873,10 @@
         <v>node teleosHeader  bluebonnetnursing.com 830-780-3944</v>
       </c>
       <c r="G7" t="s">
-        <v>642</v>
-      </c>
-      <c r="H7" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -8868,10 +8894,10 @@
         <v>node teleosHeader  brownwoodrehab.com 325-643-9555</v>
       </c>
       <c r="G8" t="s">
-        <v>642</v>
-      </c>
-      <c r="H8" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -8889,10 +8915,10 @@
         <v>node teleosHeader  buenavidanursing.com 432-362-2583</v>
       </c>
       <c r="G9" t="s">
-        <v>642</v>
-      </c>
-      <c r="H9" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -8910,10 +8936,10 @@
         <v>node teleosHeader  buenavidasanantonio.com 210-333-6815</v>
       </c>
       <c r="G10" t="s">
-        <v>642</v>
-      </c>
-      <c r="H10" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -8931,10 +8957,10 @@
         <v>node teleosHeader  caprocknursing.com 806-274-9600</v>
       </c>
       <c r="G11" t="s">
-        <v>642</v>
-      </c>
-      <c r="H11" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -8952,10 +8978,10 @@
         <v>node teleosHeader  carenursingcenter.com 325-646-5521</v>
       </c>
       <c r="G12" t="s">
-        <v>642</v>
-      </c>
-      <c r="H12" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -8973,10 +8999,10 @@
         <v>node teleosHeader  castlepinesatlufkin.com 936-699-2544</v>
       </c>
       <c r="G13" t="s">
-        <v>642</v>
-      </c>
-      <c r="H13" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -8994,10 +9020,10 @@
         <v>node teleosHeader  cedarcreeknursing.com 830-460-3767</v>
       </c>
       <c r="G14" t="s">
-        <v>642</v>
-      </c>
-      <c r="H14" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -9015,10 +9041,10 @@
         <v>node teleosHeader  centraltexasnursing.com 325-365-2538</v>
       </c>
       <c r="G15" t="s">
-        <v>642</v>
-      </c>
-      <c r="H15" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -9036,10 +9062,10 @@
         <v>node teleosHeader  cherokeerosenursing.com 254-897-7361</v>
       </c>
       <c r="G16" t="s">
-        <v>642</v>
-      </c>
-      <c r="H16" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -9057,10 +9083,10 @@
         <v>node teleosHeader  conchohealthandrehab.com 325-869-5531</v>
       </c>
       <c r="G17" t="s">
-        <v>642</v>
-      </c>
-      <c r="H17" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -9078,10 +9104,10 @@
         <v>node teleosHeader  cottonwoodnursing.com 940-387-6656</v>
       </c>
       <c r="G18" t="s">
-        <v>642</v>
-      </c>
-      <c r="H18" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -9099,10 +9125,10 @@
         <v>node teleosHeader  countryviewnr.com 972-524-2503</v>
       </c>
       <c r="G19" t="s">
-        <v>642</v>
-      </c>
-      <c r="H19" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -9120,10 +9146,10 @@
         <v>node teleosHeader  crossroadsnursingandrehab.com 979-280-0440</v>
       </c>
       <c r="G20" t="s">
-        <v>642</v>
-      </c>
-      <c r="H20" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -9141,10 +9167,10 @@
         <v>node teleosHeader  deeringsnursing.com 432-332-0371</v>
       </c>
       <c r="G21" t="s">
-        <v>642</v>
-      </c>
-      <c r="H21" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -9162,10 +9188,10 @@
         <v>node teleosHeader  deleonnursing.com 254-893-2075</v>
       </c>
       <c r="G22" t="s">
-        <v>642</v>
-      </c>
-      <c r="H22" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -9183,10 +9209,10 @@
         <v>node teleosHeader  devinehealthandrehab.com 830-663-4451</v>
       </c>
       <c r="G23" t="s">
-        <v>642</v>
-      </c>
-      <c r="H23" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -9204,10 +9230,10 @@
         <v>node teleosHeader  dogwoodtrails.com 409-283-8147</v>
       </c>
       <c r="G24" t="s">
-        <v>642</v>
-      </c>
-      <c r="H24" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -9225,10 +9251,10 @@
         <v>node teleosHeader  eaglepassnursing.com 830-773-4488</v>
       </c>
       <c r="G25" t="s">
-        <v>642</v>
-      </c>
-      <c r="H25" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -9246,10 +9272,10 @@
         <v>node teleosHeader  fairfieldnursingandrehab.com 903-389-1236</v>
       </c>
       <c r="G26" t="s">
-        <v>642</v>
-      </c>
-      <c r="H26" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -9267,10 +9293,10 @@
         <v>node teleosHeader  fivepointsnursing.com 806-356-0700</v>
       </c>
       <c r="G27" t="s">
-        <v>642</v>
-      </c>
-      <c r="H27" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -9278,17 +9304,20 @@
         <v>188</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>191</v>
+        <v>642</v>
       </c>
       <c r="D28" t="s">
         <v>188</v>
       </c>
       <c r="F28" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  www.FivePointsDeSoto.com 972-694-9810</v>
+        <v>node teleosHeader  FivePointsDeSoto.com 972-694-9810</v>
       </c>
       <c r="G28" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -9306,10 +9335,10 @@
         <v>node teleosHeader  fortressnursing.com 979-694-2200</v>
       </c>
       <c r="G29" t="s">
-        <v>642</v>
-      </c>
-      <c r="H29" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -9327,10 +9356,10 @@
         <v>node teleosHeader  franklinheightsnursing.com 915-584-9417</v>
       </c>
       <c r="G30" t="s">
-        <v>642</v>
-      </c>
-      <c r="H30" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -9348,10 +9377,10 @@
         <v>node teleosHeader  franklincare.com 979-828-5152</v>
       </c>
       <c r="G31" t="s">
-        <v>642</v>
-      </c>
-      <c r="H31" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -9369,10 +9398,10 @@
         <v>node teleosHeader  georgiamanornursing.com 806-355-6517</v>
       </c>
       <c r="G32" t="s">
-        <v>642</v>
-      </c>
-      <c r="H32" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -9390,10 +9419,10 @@
         <v>node teleosHeader  gilmernursing.com 903-843-5529</v>
       </c>
       <c r="G33" t="s">
-        <v>642</v>
-      </c>
-      <c r="H33" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -9411,8 +9440,9 @@
         <v>node teleosHeader  grahamoakscare.com 940-549-8787</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>642</v>
-      </c>
+        <v>639</v>
+      </c>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
@@ -9429,10 +9459,10 @@
         <v>node teleosHeader  granburycarecenter.com 817-573-3726</v>
       </c>
       <c r="G35" t="s">
-        <v>642</v>
-      </c>
-      <c r="H35" t="s">
-        <v>644</v>
+        <v>639</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -9450,10 +9480,10 @@
         <v>node teleosHeader  greatplainsnursing.com 806-935-4143</v>
       </c>
       <c r="G36" t="s">
-        <v>642</v>
-      </c>
-      <c r="H36" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -9471,7 +9501,10 @@
         <v>node teleosHeader  greenbrierofpalestine.com 903-729-6024</v>
       </c>
       <c r="G37" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -9489,7 +9522,10 @@
         <v>node teleosHeader  greenbrieroftyler.com 903-593-6441</v>
       </c>
       <c r="G38" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -9507,7 +9543,10 @@
         <v>node teleosHeader  greenhillvillas.com 903-572-0974</v>
       </c>
       <c r="G39" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -9525,7 +9564,10 @@
         <v>node teleosHeader  grovetonnursinghome.com 936-642-1221</v>
       </c>
       <c r="G40" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -9543,7 +9585,10 @@
         <v>node teleosHeader  heritagehousenursing.com 254-583-7904</v>
       </c>
       <c r="G41" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -9561,205 +9606,244 @@
         <v>node teleosHeader  heritageplacedecatur.com 940-627-5444</v>
       </c>
       <c r="G42" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>602</v>
+        <v>278</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>603</v>
+        <v>281</v>
       </c>
       <c r="D43" t="s">
-        <v>638</v>
+        <v>278</v>
       </c>
       <c r="F43" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  hillsidenursing.com 409-787-5300</v>
+        <v>node teleosHeader  huebnercreekhealth.com 210-691-3111</v>
+      </c>
+      <c r="G43" t="s">
+        <v>639</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="D44" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="F44" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  huebnercreekhealth.com 210-691-3111</v>
+        <v>node teleosHeader  kempcarecenter.com 903-498-8073</v>
       </c>
       <c r="G44" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="D45" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="F45" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  kempcarecenter.com 903-498-8073</v>
+        <v>node teleosHeader  kenedyhealth.com 830-583-9101</v>
       </c>
       <c r="G45" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H45" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>295</v>
+        <v>602</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>298</v>
+        <v>603</v>
       </c>
       <c r="D46" t="s">
-        <v>295</v>
+        <v>602</v>
       </c>
       <c r="F46" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  kenedyhealth.com 830-583-9101</v>
+        <v>node teleosHeader  kerenscare.com 903-396-3211</v>
       </c>
       <c r="G46" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>604</v>
+        <v>304</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>605</v>
+        <v>307</v>
       </c>
       <c r="D47" t="s">
-        <v>604</v>
+        <v>568</v>
       </c>
       <c r="F47" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  kerenscare.com 903-396-3211</v>
+        <v>node teleosHeader  labahianursing.com 361-645-8902</v>
       </c>
       <c r="G47" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D48" t="s">
-        <v>568</v>
+        <v>310</v>
       </c>
       <c r="F48" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  labahianursing.com 361-645-8902</v>
+        <v>node teleosHeader  lahaciendarehabcare.com 830-213-8138</v>
       </c>
       <c r="G48" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="D49" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="F49" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  lahaciendarehabcare.com 830-213-8138</v>
+        <v>node teleosHeader  lavidaserenanursing.com 830-774-0698</v>
       </c>
       <c r="G49" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>320</v>
+        <v>604</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>323</v>
+        <v>605</v>
       </c>
       <c r="D50" t="s">
-        <v>320</v>
+        <v>636</v>
       </c>
       <c r="F50" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  lavidaserenanursing.com 830-774-0698</v>
+        <v>node teleosHeader  lakelodgenursing.com 817-237-7231</v>
       </c>
       <c r="G50" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D51" t="s">
+        <v>328</v>
+      </c>
+      <c r="F51" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>node teleosHeader  lampstandnursing.com 979-822-6611</v>
+      </c>
+      <c r="G51" t="s">
+        <v>639</v>
+      </c>
+      <c r="H51" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D52" t="s">
+        <v>336</v>
+      </c>
+      <c r="F52" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>node teleosHeader  lubbockcarecenter.com 806-793-3252</v>
+      </c>
+      <c r="G52" t="s">
+        <v>639</v>
+      </c>
+      <c r="H52" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
         <v>606</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B53" s="8" t="s">
         <v>607</v>
       </c>
-      <c r="D51" t="s">
-        <v>639</v>
-      </c>
-      <c r="F51" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>node teleosHeader  lakelodgenursing.com 817-237-7231</v>
-      </c>
-      <c r="G51" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="D52" t="s">
-        <v>328</v>
-      </c>
-      <c r="F52" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>node teleosHeader  lampstandnursing.com 979-822-6611</v>
-      </c>
-      <c r="G52" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>339</v>
-      </c>
       <c r="D53" t="s">
-        <v>336</v>
+        <v>606</v>
       </c>
       <c r="F53" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  lubbockcarecenter.com 806-793-3252</v>
+        <v>node teleosHeader  madisonvillecarecenter.com 936-348-2735</v>
       </c>
       <c r="G53" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
         <v>608</v>
       </c>
@@ -9767,71 +9851,83 @@
         <v>609</v>
       </c>
       <c r="D54" t="s">
-        <v>608</v>
+        <v>637</v>
       </c>
       <c r="F54" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  madisonvillecarecenter.com 936-348-2735</v>
+        <v>node teleosHeader  marinecreeknursing.com 817-624-6164</v>
       </c>
       <c r="G54" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="D55" t="s">
+        <v>345</v>
+      </c>
+      <c r="F55" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>node teleosHeader  mcleancarecenter.com 806-779-2469</v>
+      </c>
+      <c r="G55" t="s">
+        <v>639</v>
+      </c>
+      <c r="H55" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D56" t="s">
+        <v>355</v>
+      </c>
+      <c r="F56" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>node teleosHeader  memphisconvalescent.com 806-259-3566</v>
+      </c>
+      <c r="G56" t="s">
+        <v>639</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
         <v>610</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="D55" t="s">
-        <v>640</v>
-      </c>
-      <c r="F55" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>node teleosHeader  marinecreeknursing.com 817-624-6164</v>
-      </c>
-      <c r="G55" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="D56" t="s">
-        <v>345</v>
-      </c>
-      <c r="F56" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>node teleosHeader  mcleancarecenter.com 806-779-2469</v>
-      </c>
-      <c r="G56" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>358</v>
-      </c>
       <c r="D57" t="s">
-        <v>355</v>
+        <v>610</v>
       </c>
       <c r="F57" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  memphisconvalescent.com 806-259-3566</v>
+        <v>node teleosHeader  mesavistahealthcenter.com 210-321-5200</v>
       </c>
       <c r="G57" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
         <v>612</v>
       </c>
@@ -9843,553 +9939,640 @@
       </c>
       <c r="F58" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  mesavistahealthcenter.com 210-321-5200</v>
+        <v>node teleosHeader  mineralwellsnursing.com 940-325-1358</v>
       </c>
       <c r="G58" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H58" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="D59" t="s">
+        <v>569</v>
+      </c>
+      <c r="F59" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>node teleosHeader  missionridgerehab.com 361-526-9223</v>
+      </c>
+      <c r="G59" t="s">
+        <v>639</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D60" t="s">
+        <v>371</v>
+      </c>
+      <c r="F60" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>node teleosHeader  mountainviewnursing.com 915-544-2002</v>
+      </c>
+      <c r="G60" t="s">
+        <v>639</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
         <v>614</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>615</v>
       </c>
-      <c r="D59" t="s">
-        <v>614</v>
-      </c>
-      <c r="F59" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>node teleosHeader  mineralwellsnursing.com 940-325-1358</v>
-      </c>
-      <c r="G59" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="D60" t="s">
-        <v>569</v>
-      </c>
-      <c r="F60" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>node teleosHeader  missionridgerehab.com 361-526-9223</v>
-      </c>
-      <c r="G60" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>374</v>
-      </c>
       <c r="D61" t="s">
-        <v>371</v>
+        <v>638</v>
       </c>
       <c r="F61" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  mountainviewnursing.com 915-544-2002</v>
+        <v>node teleosHeader  navasotanursing.com 936-825-6463</v>
       </c>
       <c r="G61" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H61" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>616</v>
+        <v>381</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>617</v>
+        <v>384</v>
       </c>
       <c r="D62" t="s">
-        <v>641</v>
+        <v>570</v>
       </c>
       <c r="F62" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  navasotanursing.com 936-825-6463</v>
+        <v>node teleosHeader  northpointenursing.com 817-498-7220</v>
       </c>
       <c r="G62" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="D63" t="s">
-        <v>570</v>
+        <v>388</v>
       </c>
       <c r="F63" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  northpointenursing.com 817-498-7220</v>
+        <v>node teleosHeader  oakridgemanornursing.com 325-643-2746</v>
       </c>
       <c r="G63" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="D64" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="F64" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  oakridgemanornursing.com 325-643-2746</v>
+        <v>node teleosHeader  oasisnursing.com 915-859-1650</v>
       </c>
       <c r="G64" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H64" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="D65" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="F65" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>node teleosHeader  oasisnursing.com 915-859-1650</v>
+        <v>node teleosHeader  pebblenursing.com 915-857-0071</v>
       </c>
       <c r="G65" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H65" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="D66" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="F66" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>node teleosHeader  pebblenursing.com 915-857-0071</v>
+        <f t="shared" ref="F66:F93" si="1">"node teleosHeader  "&amp;B66&amp;" "&amp;D66</f>
+        <v>node teleosHeader  pinetreenursing.com 903-759-3994</v>
       </c>
       <c r="G66" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H66" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="D67" t="s">
-        <v>411</v>
+        <v>571</v>
       </c>
       <c r="F67" s="20" t="str">
-        <f t="shared" ref="F67:F94" si="1">"node teleosHeader  "&amp;B67&amp;" "&amp;D67</f>
-        <v>node teleosHeader  pinetreenursing.com 903-759-3994</v>
+        <f t="shared" si="1"/>
+        <v>node teleosHeader  refugionursing.com 361-526-4641</v>
       </c>
       <c r="G67" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H67" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="D68" t="s">
-        <v>571</v>
+        <v>424</v>
       </c>
       <c r="F68" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  refugionursing.com 361-526-4641</v>
+        <v>node teleosHeader  riverccc.com 210-226-6397</v>
       </c>
       <c r="G68" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="D69" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="F69" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  riverccc.com 210-226-6397</v>
+        <v>node teleosHeader  https://rockcreekhealth.com 903-439-0107</v>
       </c>
       <c r="G69" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H69" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="D70" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="F70" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  https://rockcreekhealth.com 903-439-0107</v>
+        <v>node teleosHeader  sansabarehab.com 325-387-8123</v>
       </c>
       <c r="G70" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H70" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="D71" t="s">
-        <v>444</v>
+        <v>572</v>
       </c>
       <c r="F71" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  sansabarehab.com 325-387-8123</v>
+        <v>node teleosHeader  sevenoaksnursing.com 903-583-2191</v>
       </c>
       <c r="G71" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H71" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="D72" t="s">
-        <v>572</v>
+        <v>459</v>
       </c>
       <c r="F72" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  sevenoaksnursing.com 903-583-2191</v>
+        <v>node teleosHeader  siennanursing.com 432-333-4511</v>
       </c>
       <c r="G72" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+      <c r="H72" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="D73" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="F73" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  siennanursing.com 432-333-4511</v>
+        <v>node teleosHeader  silvertreenursing.com 210-566-9100</v>
       </c>
       <c r="G73" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+      <c r="H73" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="D74" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="F74" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  silvertreenursing.com 210-566-9100</v>
+        <v>node teleosHeader  skilledcareofmexia.com 254-472-0630</v>
       </c>
       <c r="G74" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+      <c r="H74" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="D75" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="F75" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  skilledcareofmexia.com 254-472-0630</v>
+        <v>node teleosHeader  slatoncarecenter.com 806-828-6268</v>
       </c>
       <c r="G75" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+      <c r="H75" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>486</v>
+        <v>616</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>489</v>
+        <v>617</v>
       </c>
       <c r="D76" t="s">
-        <v>486</v>
+        <v>616</v>
       </c>
       <c r="F76" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  slatoncarecenter.com 806-828-6268</v>
+        <v>node teleosHeader  songbirdnursing.com 325-646-4750</v>
       </c>
       <c r="G76" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="15" t="s">
+        <v>640</v>
+      </c>
+      <c r="H76" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
         <v>618</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="18" t="s">
         <v>619</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="19" t="s">
         <v>618</v>
       </c>
       <c r="F77" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  songbirdnursing.com 325-646-4750</v>
-      </c>
-      <c r="G77" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="17" t="s">
-        <v>620</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>621</v>
-      </c>
-      <c r="D78" s="19" t="s">
-        <v>620</v>
+        <v>node teleosHeader  southernspecialtynursing.com 806-795-1774</v>
+      </c>
+      <c r="G77" s="19" t="s">
+        <v>640</v>
+      </c>
+      <c r="H77" s="22"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="15" t="s">
+        <v>493</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="D78" t="s">
+        <v>493</v>
       </c>
       <c r="F78" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  southernspecialtynursing.com 806-795-1774</v>
-      </c>
-      <c r="G78" s="19" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="15" t="s">
-        <v>493</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>496</v>
-      </c>
-      <c r="D79" t="s">
-        <v>493</v>
+        <v>node teleosHeader  stgilesnursing.com 915-859-3010</v>
+      </c>
+      <c r="G78" t="s">
+        <v>640</v>
+      </c>
+      <c r="H78" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>621</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>620</v>
       </c>
       <c r="F79" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  stgilesnursing.com 915-859-3010</v>
-      </c>
-      <c r="G79" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="17" t="s">
-        <v>622</v>
-      </c>
-      <c r="B80" s="18" t="s">
-        <v>623</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>622</v>
+        <v>node teleosHeader  stteresanursing.com 915-595-6137</v>
+      </c>
+      <c r="G79" s="19" t="s">
+        <v>640</v>
+      </c>
+      <c r="H79" s="22"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="D80" t="s">
+        <v>500</v>
       </c>
       <c r="F80" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  stteresanursing.com 915-595-6137</v>
-      </c>
-      <c r="G80" s="19" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+        <v>node teleosHeader  sunflowerparkhealth.com 972-932-7776</v>
+      </c>
+      <c r="G80" t="s">
+        <v>640</v>
+      </c>
+      <c r="H80" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
       <c r="D81" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="F81" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  sunflowerparkhealth.com 972-932-7776</v>
+        <v>node teleosHeader  thearborsnursing.com 903-683-1042</v>
       </c>
       <c r="G81" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+      <c r="H81" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="D82" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c r="F82" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  thearborsnursing.com 903-683-1042</v>
+        <v>node teleosHeader  atriumofbellmead.com 254-296-8976</v>
       </c>
       <c r="G82" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+      <c r="H82" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="D83" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="F83" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  atriumofbellmead.com 254-296-8976</v>
+        <v>node teleosHeader  https://hillsnursing.com 940-627-2165</v>
       </c>
       <c r="G83" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+      <c r="H83" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>525</v>
+        <v>535</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="D84" t="s">
-        <v>525</v>
+        <v>573</v>
       </c>
       <c r="F84" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  https://hillsnursing.com 940-627-2165</v>
+        <v>node teleosHeader  premierofalice.com 361-666-3800</v>
       </c>
       <c r="G84" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="15" t="s">
-        <v>535</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="D85" t="s">
-        <v>573</v>
+        <v>639</v>
+      </c>
+      <c r="H84" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>623</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>622</v>
       </c>
       <c r="F85" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  premierofalice.com 361-666-3800</v>
-      </c>
-      <c r="G85" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="17" t="s">
-        <v>624</v>
-      </c>
-      <c r="B86" s="18" t="s">
-        <v>625</v>
-      </c>
-      <c r="D86" s="19" t="s">
-        <v>624</v>
+        <v>node teleosHeader  rioatmissiontrails.com 210-531-0569</v>
+      </c>
+      <c r="G85" s="19" t="s">
+        <v>640</v>
+      </c>
+      <c r="H85" s="22"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="D86" t="s">
+        <v>542</v>
       </c>
       <c r="F86" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  rioatmissiontrails.com 210-531-0569</v>
-      </c>
-      <c r="G86" s="19" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+        <v>node teleosHeader  twinoakscare.com 903-586-9031</v>
+      </c>
+      <c r="G86" t="s">
+        <v>640</v>
+      </c>
+      <c r="H86" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>545</v>
+        <v>554</v>
       </c>
       <c r="D87" t="s">
-        <v>542</v>
+        <v>574</v>
       </c>
       <c r="F87" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  twinoakscare.com 903-586-9031</v>
+        <v>node teleosHeader  universityparknr.com 940-692-8001</v>
       </c>
       <c r="G87" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H87" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
-        <v>551</v>
+        <v>624</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>554</v>
+        <v>625</v>
       </c>
       <c r="D88" t="s">
-        <v>574</v>
+        <v>624</v>
       </c>
       <c r="F88" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  universityparknr.com 940-692-8001</v>
+        <v>node teleosHeader  vidorhealth.com 409-769-2454</v>
       </c>
       <c r="G88" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H88" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="s">
         <v>626</v>
       </c>
@@ -10401,13 +10584,16 @@
       </c>
       <c r="F89" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  vidorhealth.com 409-769-2454</v>
+        <v>node teleosHeader  villatoscanarehab.com 281-586-6088</v>
       </c>
       <c r="G89" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H89" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
         <v>628</v>
       </c>
@@ -10419,49 +10605,58 @@
       </c>
       <c r="F90" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  villatoscanarehab.com 281-586-6088</v>
+        <v>node teleosHeader  wellingtoncarecenter.com 806-447-2513</v>
       </c>
       <c r="G90" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H90" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>630</v>
+        <v>559</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>631</v>
+        <v>562</v>
       </c>
       <c r="D91" t="s">
-        <v>630</v>
+        <v>575</v>
       </c>
       <c r="F91" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  wellingtoncarecenter.com 806-447-2513</v>
+        <v>node teleosHeader  Westwardtrailsnursing.com/ 936-569-2631</v>
       </c>
       <c r="G91" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H91" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>559</v>
+        <v>630</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>562</v>
+        <v>631</v>
       </c>
       <c r="D92" t="s">
-        <v>575</v>
+        <v>630</v>
       </c>
       <c r="F92" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  Westwardtrailsnursing.com/ 936-569-2631</v>
+        <v>node teleosHeader  whisperingpinescare.com 903-757-8786</v>
       </c>
       <c r="G92" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+      <c r="H92" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
         <v>632</v>
       </c>
@@ -10473,28 +10668,13 @@
       </c>
       <c r="F93" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>node teleosHeader  whisperingpinescare.com 903-757-8786</v>
+        <v>node teleosHeader  whisperwoodnursing.com 806-793-1111</v>
       </c>
       <c r="G93" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="15" t="s">
-        <v>634</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>635</v>
-      </c>
-      <c r="D94" t="s">
-        <v>634</v>
-      </c>
-      <c r="F94" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v>node teleosHeader  whisperwoodnursing.com 806-793-1111</v>
-      </c>
-      <c r="G94" t="s">
-        <v>642</v>
+        <v>639</v>
+      </c>
+      <c r="H93" s="21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -10539,59 +10719,1572 @@
     <hyperlink ref="B40" r:id="rId38" display="http://grovetonnursinghome.com/" xr:uid="{FCB3F756-99E7-3F4D-AB92-B814EAD225F7}"/>
     <hyperlink ref="B41" r:id="rId39" display="http://heritagehousenursing.com/" xr:uid="{E870D705-C847-D749-88D1-488D33B502EC}"/>
     <hyperlink ref="B42" r:id="rId40" display="http://heritageplacedecatur.com/" xr:uid="{EE04EDAD-756F-3A4B-9C79-1FC6C2A3C143}"/>
-    <hyperlink ref="B43" r:id="rId41" display="http://hillsidenursing.com/" xr:uid="{A6FA5A20-BA23-544E-999D-C24A97D2C9A4}"/>
-    <hyperlink ref="B44" r:id="rId42" display="http://huebnercreekhealth.com/" xr:uid="{C48607DD-3ED6-2647-A858-5672AEDA1458}"/>
-    <hyperlink ref="B45" r:id="rId43" display="http://kempcarecenter.com/" xr:uid="{39243DE7-132A-4D4D-B9C7-63764037AB90}"/>
-    <hyperlink ref="B46" r:id="rId44" display="http://kenedyhealth.com/" xr:uid="{5D30F008-C740-D547-8714-FA663EB42032}"/>
-    <hyperlink ref="B47" r:id="rId45" display="http://kerenscare.com/" xr:uid="{A677E63D-7915-4140-BAF6-2509F23B6683}"/>
-    <hyperlink ref="B48" r:id="rId46" display="http://labahianursing.com/" xr:uid="{7F761B73-02B4-7647-8BF4-0EE6823A5176}"/>
-    <hyperlink ref="B49" r:id="rId47" display="http://lahaciendarehabcare.com/" xr:uid="{5A7DA3E4-AB34-0C4F-8160-76D83D12D910}"/>
-    <hyperlink ref="B50" r:id="rId48" display="http://lavidaserenanursing.com/" xr:uid="{7A3CE978-F42B-4340-B18F-D855BAC146CB}"/>
-    <hyperlink ref="B51" r:id="rId49" display="http://lakelodgenursing.com/" xr:uid="{54BC9ACB-4A4C-CE44-AFB3-B0C25912F354}"/>
-    <hyperlink ref="B52" r:id="rId50" display="http://lampstandnursing.com/" xr:uid="{C9946672-73FC-A04F-9520-989731185C47}"/>
-    <hyperlink ref="B53" r:id="rId51" display="http://lubbockcarecenter.com/" xr:uid="{3370374E-1ED5-2049-87AB-C5AF77295879}"/>
-    <hyperlink ref="B54" r:id="rId52" display="http://madisonvillecarecenter.com/" xr:uid="{B4F8D9C9-2121-4145-B5D4-6C991AEFBA22}"/>
-    <hyperlink ref="B55" r:id="rId53" display="http://marinecreeknursing.com/" xr:uid="{4F8E56EA-DB57-1644-8711-100CFA133267}"/>
-    <hyperlink ref="B56" r:id="rId54" display="http://mcleancarecenter.com/" xr:uid="{BC4815D3-23BC-274F-9AD1-38DADD094EBD}"/>
-    <hyperlink ref="B57" r:id="rId55" display="http://memphisconvalescent.com/" xr:uid="{0FB8A03C-F1DC-834A-A072-F8695131DC2E}"/>
-    <hyperlink ref="B58" r:id="rId56" display="http://mesavistahealthcenter.com/" xr:uid="{0846981E-E8D1-B643-A590-287B55BB20ED}"/>
-    <hyperlink ref="B59" r:id="rId57" display="http://mineralwellsnursing.com/" xr:uid="{82AF773F-4454-EC46-AFD0-BBD29A991969}"/>
-    <hyperlink ref="B60" r:id="rId58" display="http://missionridgerehab.com/" xr:uid="{6FED89F1-07C1-124E-8E88-FF0680FB723E}"/>
-    <hyperlink ref="B61" r:id="rId59" display="http://mountainviewnursing.com/" xr:uid="{259C48D9-9669-F544-A97F-E7CA4A88D84A}"/>
-    <hyperlink ref="B62" r:id="rId60" display="http://navasotanursing.com/" xr:uid="{531910E7-8AB8-A143-974A-54AD440FD397}"/>
-    <hyperlink ref="B63" r:id="rId61" display="http://northpointenursing.com/" xr:uid="{11668ACE-8F6A-E243-BCAE-B7DA80BF9B4C}"/>
-    <hyperlink ref="B64" r:id="rId62" display="http://oakridgemanornursing.com/" xr:uid="{86690633-5AB1-4948-AF83-ECF80D0C7791}"/>
-    <hyperlink ref="B65" r:id="rId63" display="http://oasisnursing.com/" xr:uid="{6373D5CC-B914-BB42-8D08-A4A70DE1592E}"/>
-    <hyperlink ref="B66" r:id="rId64" display="http://pebblenursing.com/" xr:uid="{115E8F92-EC49-FC42-9D2E-1F9182A6A21E}"/>
-    <hyperlink ref="B67" r:id="rId65" display="http://pinetreenursing.com/" xr:uid="{FB7F3D05-2C2D-3444-A76E-31D0275D6A20}"/>
-    <hyperlink ref="B68" r:id="rId66" display="http://refugionursing.com/" xr:uid="{8B23AEFC-E69F-1A49-8429-6A65977B3D3F}"/>
-    <hyperlink ref="B69" r:id="rId67" display="http://riverccc.com/" xr:uid="{5D0B88CE-41A7-4B4C-9958-04363B25354B}"/>
-    <hyperlink ref="B70" r:id="rId68" display="https://rockcreekhealth.com/" xr:uid="{3A40D940-9216-A44D-9883-BB839A7332CF}"/>
-    <hyperlink ref="B71" r:id="rId69" display="http://sansabarehab.com/" xr:uid="{DF97630E-AC0E-2442-AD70-246C23E7ED37}"/>
-    <hyperlink ref="B72" r:id="rId70" display="http://sevenoaksnursing.com/" xr:uid="{2D8DEB30-79B6-1244-85E5-9A946CC5A0FB}"/>
-    <hyperlink ref="B73" r:id="rId71" display="http://siennanursing.com/" xr:uid="{F7EBFD24-519D-3945-8BF6-262603BD3FBD}"/>
-    <hyperlink ref="B74" r:id="rId72" display="http://silvertreenursing.com/" xr:uid="{87E754BC-BAC0-C044-94AA-2F751438ADEB}"/>
-    <hyperlink ref="B75" r:id="rId73" display="http://skilledcareofmexia.com/" xr:uid="{FFE9709B-E73F-A344-8A0C-C840B5169E7E}"/>
-    <hyperlink ref="B76" r:id="rId74" display="http://slatoncarecenter.com/" xr:uid="{2670C454-FDAF-7B4E-AC2E-C8C0BB861CC4}"/>
-    <hyperlink ref="B77" r:id="rId75" display="http://songbirdnursing.com/" xr:uid="{42B4C7B2-2358-1944-9D7C-ABF7445B30FD}"/>
-    <hyperlink ref="B78" r:id="rId76" display="http://southernspecialtynursing.com/" xr:uid="{9CB98944-7DF6-DA4D-812B-F8258ED5B1D6}"/>
-    <hyperlink ref="B79" r:id="rId77" display="http://stgilesnursing.com/" xr:uid="{DB5DC2FF-2B36-A343-BB9F-B39376966C3E}"/>
-    <hyperlink ref="B80" r:id="rId78" display="http://stteresanursing.com/" xr:uid="{1308AC42-21A5-6B4E-A01A-7818B764A2D4}"/>
-    <hyperlink ref="B81" r:id="rId79" display="http://sunflowerparkhealth.com/" xr:uid="{59AB1513-9525-5344-919B-93E680A619D4}"/>
-    <hyperlink ref="B82" r:id="rId80" display="http://thearborsnursing.com/" xr:uid="{EBF0E3D2-43F7-424D-BC47-41EDFAB140FC}"/>
-    <hyperlink ref="B83" r:id="rId81" display="http://atriumofbellmead.com/" xr:uid="{0A74E92B-82C9-2A4A-AF73-AEAAB1707D7D}"/>
-    <hyperlink ref="B84" r:id="rId82" display="https://hillsnursing.com/" xr:uid="{71307966-18A9-BB45-90EE-0A0334BFB483}"/>
-    <hyperlink ref="B85" r:id="rId83" display="http://premierofalice.com/" xr:uid="{17D04C15-0535-914F-8F42-0C548E071AB2}"/>
-    <hyperlink ref="B86" r:id="rId84" display="http://rioatmissiontrails.com/" xr:uid="{0E6109BE-591B-434F-9584-6BB2F850515C}"/>
-    <hyperlink ref="B87" r:id="rId85" display="http://twinoakscare.com/" xr:uid="{E8D1784D-CD38-F64A-B9C3-45E86B1F3D14}"/>
-    <hyperlink ref="B88" r:id="rId86" display="http://universityparknr.com/" xr:uid="{40DB499A-9F13-FA4D-AF60-CB249207DFE6}"/>
-    <hyperlink ref="B89" r:id="rId87" display="http://vidorhealth.com/" xr:uid="{F64FC8EE-BAB5-2348-80DB-D30077BC82C9}"/>
-    <hyperlink ref="B90" r:id="rId88" display="http://villatoscanarehab.com/" xr:uid="{EA6457A6-05A5-5246-9B4C-A46873F674B5}"/>
-    <hyperlink ref="B91" r:id="rId89" display="http://wellingtoncarecenter.com/" xr:uid="{0E93126C-198C-2E42-BE14-C02780F8730C}"/>
-    <hyperlink ref="B92" r:id="rId90" display="http://westwardtrailsnursing.com/" xr:uid="{E53C3D85-8B80-3B48-82AB-25CCA3EA3310}"/>
-    <hyperlink ref="B93" r:id="rId91" display="http://whisperingpinescare.com/" xr:uid="{98C33324-F0BF-F043-BBE3-6D50B2C86DC1}"/>
-    <hyperlink ref="B94" r:id="rId92" display="http://whisperwoodnursing.com/" xr:uid="{50D9CE99-D3C6-2149-A31E-CA0FC2C4AC96}"/>
-    <hyperlink ref="B34" r:id="rId93" display="http://grahamoakscare.com/" xr:uid="{0D8F6B4B-DB2B-B047-B336-067C981555B7}"/>
+    <hyperlink ref="B43" r:id="rId41" display="http://huebnercreekhealth.com/" xr:uid="{C48607DD-3ED6-2647-A858-5672AEDA1458}"/>
+    <hyperlink ref="B44" r:id="rId42" display="http://kempcarecenter.com/" xr:uid="{39243DE7-132A-4D4D-B9C7-63764037AB90}"/>
+    <hyperlink ref="B45" r:id="rId43" display="http://kenedyhealth.com/" xr:uid="{5D30F008-C740-D547-8714-FA663EB42032}"/>
+    <hyperlink ref="B46" r:id="rId44" display="http://kerenscare.com/" xr:uid="{A677E63D-7915-4140-BAF6-2509F23B6683}"/>
+    <hyperlink ref="B47" r:id="rId45" display="http://labahianursing.com/" xr:uid="{7F761B73-02B4-7647-8BF4-0EE6823A5176}"/>
+    <hyperlink ref="B48" r:id="rId46" display="http://lahaciendarehabcare.com/" xr:uid="{5A7DA3E4-AB34-0C4F-8160-76D83D12D910}"/>
+    <hyperlink ref="B49" r:id="rId47" display="http://lavidaserenanursing.com/" xr:uid="{7A3CE978-F42B-4340-B18F-D855BAC146CB}"/>
+    <hyperlink ref="B50" r:id="rId48" display="http://lakelodgenursing.com/" xr:uid="{54BC9ACB-4A4C-CE44-AFB3-B0C25912F354}"/>
+    <hyperlink ref="B51" r:id="rId49" display="http://lampstandnursing.com/" xr:uid="{C9946672-73FC-A04F-9520-989731185C47}"/>
+    <hyperlink ref="B52" r:id="rId50" display="http://lubbockcarecenter.com/" xr:uid="{3370374E-1ED5-2049-87AB-C5AF77295879}"/>
+    <hyperlink ref="B53" r:id="rId51" display="http://madisonvillecarecenter.com/" xr:uid="{B4F8D9C9-2121-4145-B5D4-6C991AEFBA22}"/>
+    <hyperlink ref="B54" r:id="rId52" display="http://marinecreeknursing.com/" xr:uid="{4F8E56EA-DB57-1644-8711-100CFA133267}"/>
+    <hyperlink ref="B55" r:id="rId53" display="http://mcleancarecenter.com/" xr:uid="{BC4815D3-23BC-274F-9AD1-38DADD094EBD}"/>
+    <hyperlink ref="B56" r:id="rId54" display="http://memphisconvalescent.com/" xr:uid="{0FB8A03C-F1DC-834A-A072-F8695131DC2E}"/>
+    <hyperlink ref="B57" r:id="rId55" display="http://mesavistahealthcenter.com/" xr:uid="{0846981E-E8D1-B643-A590-287B55BB20ED}"/>
+    <hyperlink ref="B58" r:id="rId56" display="http://mineralwellsnursing.com/" xr:uid="{82AF773F-4454-EC46-AFD0-BBD29A991969}"/>
+    <hyperlink ref="B59" r:id="rId57" display="http://missionridgerehab.com/" xr:uid="{6FED89F1-07C1-124E-8E88-FF0680FB723E}"/>
+    <hyperlink ref="B60" r:id="rId58" display="http://mountainviewnursing.com/" xr:uid="{259C48D9-9669-F544-A97F-E7CA4A88D84A}"/>
+    <hyperlink ref="B61" r:id="rId59" display="http://navasotanursing.com/" xr:uid="{531910E7-8AB8-A143-974A-54AD440FD397}"/>
+    <hyperlink ref="B62" r:id="rId60" display="http://northpointenursing.com/" xr:uid="{11668ACE-8F6A-E243-BCAE-B7DA80BF9B4C}"/>
+    <hyperlink ref="B63" r:id="rId61" display="http://oakridgemanornursing.com/" xr:uid="{86690633-5AB1-4948-AF83-ECF80D0C7791}"/>
+    <hyperlink ref="B64" r:id="rId62" display="http://oasisnursing.com/" xr:uid="{6373D5CC-B914-BB42-8D08-A4A70DE1592E}"/>
+    <hyperlink ref="B65" r:id="rId63" display="http://pebblenursing.com/" xr:uid="{115E8F92-EC49-FC42-9D2E-1F9182A6A21E}"/>
+    <hyperlink ref="B66" r:id="rId64" display="http://pinetreenursing.com/" xr:uid="{FB7F3D05-2C2D-3444-A76E-31D0275D6A20}"/>
+    <hyperlink ref="B67" r:id="rId65" display="http://refugionursing.com/" xr:uid="{8B23AEFC-E69F-1A49-8429-6A65977B3D3F}"/>
+    <hyperlink ref="B68" r:id="rId66" display="http://riverccc.com/" xr:uid="{5D0B88CE-41A7-4B4C-9958-04363B25354B}"/>
+    <hyperlink ref="B69" r:id="rId67" display="https://rockcreekhealth.com/" xr:uid="{3A40D940-9216-A44D-9883-BB839A7332CF}"/>
+    <hyperlink ref="B70" r:id="rId68" display="http://sansabarehab.com/" xr:uid="{DF97630E-AC0E-2442-AD70-246C23E7ED37}"/>
+    <hyperlink ref="B71" r:id="rId69" display="http://sevenoaksnursing.com/" xr:uid="{2D8DEB30-79B6-1244-85E5-9A946CC5A0FB}"/>
+    <hyperlink ref="B72" r:id="rId70" display="http://siennanursing.com/" xr:uid="{F7EBFD24-519D-3945-8BF6-262603BD3FBD}"/>
+    <hyperlink ref="B73" r:id="rId71" display="http://silvertreenursing.com/" xr:uid="{87E754BC-BAC0-C044-94AA-2F751438ADEB}"/>
+    <hyperlink ref="B74" r:id="rId72" display="http://skilledcareofmexia.com/" xr:uid="{FFE9709B-E73F-A344-8A0C-C840B5169E7E}"/>
+    <hyperlink ref="B75" r:id="rId73" display="http://slatoncarecenter.com/" xr:uid="{2670C454-FDAF-7B4E-AC2E-C8C0BB861CC4}"/>
+    <hyperlink ref="B76" r:id="rId74" display="http://songbirdnursing.com/" xr:uid="{42B4C7B2-2358-1944-9D7C-ABF7445B30FD}"/>
+    <hyperlink ref="B77" r:id="rId75" display="http://southernspecialtynursing.com/" xr:uid="{9CB98944-7DF6-DA4D-812B-F8258ED5B1D6}"/>
+    <hyperlink ref="B78" r:id="rId76" display="http://stgilesnursing.com/" xr:uid="{DB5DC2FF-2B36-A343-BB9F-B39376966C3E}"/>
+    <hyperlink ref="B79" r:id="rId77" display="http://stteresanursing.com/" xr:uid="{1308AC42-21A5-6B4E-A01A-7818B764A2D4}"/>
+    <hyperlink ref="B80" r:id="rId78" display="http://sunflowerparkhealth.com/" xr:uid="{59AB1513-9525-5344-919B-93E680A619D4}"/>
+    <hyperlink ref="B81" r:id="rId79" display="http://thearborsnursing.com/" xr:uid="{EBF0E3D2-43F7-424D-BC47-41EDFAB140FC}"/>
+    <hyperlink ref="B82" r:id="rId80" display="http://atriumofbellmead.com/" xr:uid="{0A74E92B-82C9-2A4A-AF73-AEAAB1707D7D}"/>
+    <hyperlink ref="B83" r:id="rId81" display="https://hillsnursing.com/" xr:uid="{71307966-18A9-BB45-90EE-0A0334BFB483}"/>
+    <hyperlink ref="B84" r:id="rId82" display="http://premierofalice.com/" xr:uid="{17D04C15-0535-914F-8F42-0C548E071AB2}"/>
+    <hyperlink ref="B85" r:id="rId83" display="http://rioatmissiontrails.com/" xr:uid="{0E6109BE-591B-434F-9584-6BB2F850515C}"/>
+    <hyperlink ref="B86" r:id="rId84" display="http://twinoakscare.com/" xr:uid="{E8D1784D-CD38-F64A-B9C3-45E86B1F3D14}"/>
+    <hyperlink ref="B87" r:id="rId85" display="http://universityparknr.com/" xr:uid="{40DB499A-9F13-FA4D-AF60-CB249207DFE6}"/>
+    <hyperlink ref="B88" r:id="rId86" display="http://vidorhealth.com/" xr:uid="{F64FC8EE-BAB5-2348-80DB-D30077BC82C9}"/>
+    <hyperlink ref="B89" r:id="rId87" display="http://villatoscanarehab.com/" xr:uid="{EA6457A6-05A5-5246-9B4C-A46873F674B5}"/>
+    <hyperlink ref="B90" r:id="rId88" display="http://wellingtoncarecenter.com/" xr:uid="{0E93126C-198C-2E42-BE14-C02780F8730C}"/>
+    <hyperlink ref="B91" r:id="rId89" display="http://westwardtrailsnursing.com/" xr:uid="{E53C3D85-8B80-3B48-82AB-25CCA3EA3310}"/>
+    <hyperlink ref="B92" r:id="rId90" display="http://whisperingpinescare.com/" xr:uid="{98C33324-F0BF-F043-BBE3-6D50B2C86DC1}"/>
+    <hyperlink ref="B93" r:id="rId91" display="http://whisperwoodnursing.com/" xr:uid="{50D9CE99-D3C6-2149-A31E-CA0FC2C4AC96}"/>
+    <hyperlink ref="B34" r:id="rId92" display="http://grahamoakscare.com/" xr:uid="{0D8F6B4B-DB2B-B047-B336-067C981555B7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47ABF03-C855-6B49-B3E9-76F035237A07}">
+  <dimension ref="A1:D92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="str">
+        <f>A1</f>
+        <v>amarilloskilledcenter.com</v>
+      </c>
+      <c r="C1" s="26" t="str">
+        <f>B1</f>
+        <v>amarilloskilledcenter.com</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:C65" si="0">A2</f>
+        <v>beaumontnursingandrehab.com</v>
+      </c>
+      <c r="C2" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>beaumontnursingandrehab.com</v>
+      </c>
+      <c r="D2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>bertramnursing.com</v>
+      </c>
+      <c r="C3" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>bertramnursing.com</v>
+      </c>
+      <c r="D3" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>bigspringcenterforskilledcare.com</v>
+      </c>
+      <c r="C4" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>bigspringcenterforskilledcare.com</v>
+      </c>
+      <c r="D4" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>581</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>birchwoodnursing.com</v>
+      </c>
+      <c r="C5" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>birchwoodnursing.com</v>
+      </c>
+      <c r="D5" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>bluebonnetnursing.com</v>
+      </c>
+      <c r="C6" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>bluebonnetnursing.com</v>
+      </c>
+      <c r="D6" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>brownwoodrehab.com</v>
+      </c>
+      <c r="C7" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>brownwoodrehab.com</v>
+      </c>
+      <c r="D7" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>buenavidanursing.com</v>
+      </c>
+      <c r="C8" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>buenavidanursing.com</v>
+      </c>
+      <c r="D8" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>583</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>buenavidasanantonio.com</v>
+      </c>
+      <c r="C9" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>buenavidasanantonio.com</v>
+      </c>
+      <c r="D9" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>caprocknursing.com</v>
+      </c>
+      <c r="C10" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>caprocknursing.com</v>
+      </c>
+      <c r="D10" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>carenursingcenter.com</v>
+      </c>
+      <c r="C11" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>carenursingcenter.com</v>
+      </c>
+      <c r="D11" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>castlepinesatlufkin.com</v>
+      </c>
+      <c r="C12" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>castlepinesatlufkin.com</v>
+      </c>
+      <c r="D12" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>cedarcreeknursing.com</v>
+      </c>
+      <c r="C13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>cedarcreeknursing.com</v>
+      </c>
+      <c r="D13" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
+        <v>585</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>centraltexasnursing.com</v>
+      </c>
+      <c r="C14" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>centraltexasnursing.com</v>
+      </c>
+      <c r="D14" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>cherokeerosenursing.com</v>
+      </c>
+      <c r="C15" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>cherokeerosenursing.com</v>
+      </c>
+      <c r="D15" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>587</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>conchohealthandrehab.com</v>
+      </c>
+      <c r="C16" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>conchohealthandrehab.com</v>
+      </c>
+      <c r="D16" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>cottonwoodnursing.com</v>
+      </c>
+      <c r="C17" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>cottonwoodnursing.com</v>
+      </c>
+      <c r="D17" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>countryviewnr.com</v>
+      </c>
+      <c r="C18" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>countryviewnr.com</v>
+      </c>
+      <c r="D18" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>crossroadsnursingandrehab.com</v>
+      </c>
+      <c r="C19" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>crossroadsnursingandrehab.com</v>
+      </c>
+      <c r="D19" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>deeringsnursing.com</v>
+      </c>
+      <c r="C20" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>deeringsnursing.com</v>
+      </c>
+      <c r="D20" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>deleonnursing.com</v>
+      </c>
+      <c r="C21" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>deleonnursing.com</v>
+      </c>
+      <c r="D21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>devinehealthandrehab.com</v>
+      </c>
+      <c r="C22" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>devinehealthandrehab.com</v>
+      </c>
+      <c r="D22" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>589</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>dogwoodtrails.com</v>
+      </c>
+      <c r="C23" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>dogwoodtrails.com</v>
+      </c>
+      <c r="D23" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>eaglepassnursing.com</v>
+      </c>
+      <c r="C24" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>eaglepassnursing.com</v>
+      </c>
+      <c r="D24" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
+        <v>591</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>fairfieldnursingandrehab.com</v>
+      </c>
+      <c r="C25" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>fairfieldnursingandrehab.com</v>
+      </c>
+      <c r="D25" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>fivepointsnursing.com</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>fivepointsnursing.com</v>
+      </c>
+      <c r="D26" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="24" t="s">
+        <v>642</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>FivePointsDeSoto.com</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>FivePointsDeSoto.com</v>
+      </c>
+      <c r="D27" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>fortressnursing.com</v>
+      </c>
+      <c r="C28" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>fortressnursing.com</v>
+      </c>
+      <c r="D28" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>franklinheightsnursing.com</v>
+      </c>
+      <c r="C29" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>franklinheightsnursing.com</v>
+      </c>
+      <c r="D29" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>franklincare.com</v>
+      </c>
+      <c r="C30" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>franklincare.com</v>
+      </c>
+      <c r="D30" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>georgiamanornursing.com</v>
+      </c>
+      <c r="C31" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>georgiamanornursing.com</v>
+      </c>
+      <c r="D31" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="24" t="s">
+        <v>593</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>gilmernursing.com</v>
+      </c>
+      <c r="C32" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>gilmernursing.com</v>
+      </c>
+      <c r="D32" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="24" t="s">
+        <v>595</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>grahamoakscare.com</v>
+      </c>
+      <c r="C33" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>grahamoakscare.com</v>
+      </c>
+      <c r="D33" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>granburycarecenter.com</v>
+      </c>
+      <c r="C34" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>granburycarecenter.com</v>
+      </c>
+      <c r="D34" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>greatplainsnursing.com</v>
+      </c>
+      <c r="C35" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>greatplainsnursing.com</v>
+      </c>
+      <c r="D35" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>greenbrierofpalestine.com</v>
+      </c>
+      <c r="C36" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>greenbrierofpalestine.com</v>
+      </c>
+      <c r="D36" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>greenbrieroftyler.com</v>
+      </c>
+      <c r="C37" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>greenbrieroftyler.com</v>
+      </c>
+      <c r="D37" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>greenhillvillas.com</v>
+      </c>
+      <c r="C38" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>greenhillvillas.com</v>
+      </c>
+      <c r="D38" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>grovetonnursinghome.com</v>
+      </c>
+      <c r="C39" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>grovetonnursinghome.com</v>
+      </c>
+      <c r="D39" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>heritagehousenursing.com</v>
+      </c>
+      <c r="C40" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>heritagehousenursing.com</v>
+      </c>
+      <c r="D40" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>heritageplacedecatur.com</v>
+      </c>
+      <c r="C41" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>heritageplacedecatur.com</v>
+      </c>
+      <c r="D41" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>huebnercreekhealth.com</v>
+      </c>
+      <c r="C42" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>huebnercreekhealth.com</v>
+      </c>
+      <c r="D42" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>kempcarecenter.com</v>
+      </c>
+      <c r="C43" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>kempcarecenter.com</v>
+      </c>
+      <c r="D43" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>kenedyhealth.com</v>
+      </c>
+      <c r="C44" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>kenedyhealth.com</v>
+      </c>
+      <c r="D44" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>kerenscare.com</v>
+      </c>
+      <c r="C45" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>kerenscare.com</v>
+      </c>
+      <c r="D45" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>labahianursing.com</v>
+      </c>
+      <c r="C46" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>labahianursing.com</v>
+      </c>
+      <c r="D46" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>lahaciendarehabcare.com</v>
+      </c>
+      <c r="C47" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>lahaciendarehabcare.com</v>
+      </c>
+      <c r="D47" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>lavidaserenanursing.com</v>
+      </c>
+      <c r="C48" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>lavidaserenanursing.com</v>
+      </c>
+      <c r="D48" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>lakelodgenursing.com</v>
+      </c>
+      <c r="C49" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>lakelodgenursing.com</v>
+      </c>
+      <c r="D49" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>lampstandnursing.com</v>
+      </c>
+      <c r="C50" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>lampstandnursing.com</v>
+      </c>
+      <c r="D50" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>lubbockcarecenter.com</v>
+      </c>
+      <c r="C51" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>lubbockcarecenter.com</v>
+      </c>
+      <c r="D51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="24" t="s">
+        <v>607</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>madisonvillecarecenter.com</v>
+      </c>
+      <c r="C52" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>madisonvillecarecenter.com</v>
+      </c>
+      <c r="D52" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="24" t="s">
+        <v>609</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>marinecreeknursing.com</v>
+      </c>
+      <c r="C53" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>marinecreeknursing.com</v>
+      </c>
+      <c r="D53" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>mcleancarecenter.com</v>
+      </c>
+      <c r="C54" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>mcleancarecenter.com</v>
+      </c>
+      <c r="D54" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>memphisconvalescent.com</v>
+      </c>
+      <c r="C55" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>memphisconvalescent.com</v>
+      </c>
+      <c r="D55" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="24" t="s">
+        <v>611</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>mesavistahealthcenter.com</v>
+      </c>
+      <c r="C56" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>mesavistahealthcenter.com</v>
+      </c>
+      <c r="D56" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="24" t="s">
+        <v>613</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>mineralwellsnursing.com</v>
+      </c>
+      <c r="C57" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>mineralwellsnursing.com</v>
+      </c>
+      <c r="D57" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>missionridgerehab.com</v>
+      </c>
+      <c r="C58" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>missionridgerehab.com</v>
+      </c>
+      <c r="D58" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>mountainviewnursing.com</v>
+      </c>
+      <c r="C59" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>mountainviewnursing.com</v>
+      </c>
+      <c r="D59" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="24" t="s">
+        <v>615</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>navasotanursing.com</v>
+      </c>
+      <c r="C60" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>navasotanursing.com</v>
+      </c>
+      <c r="D60" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>northpointenursing.com</v>
+      </c>
+      <c r="C61" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>northpointenursing.com</v>
+      </c>
+      <c r="D61" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>oakridgemanornursing.com</v>
+      </c>
+      <c r="C62" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>oakridgemanornursing.com</v>
+      </c>
+      <c r="D62" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>oasisnursing.com</v>
+      </c>
+      <c r="C63" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>oasisnursing.com</v>
+      </c>
+      <c r="D63" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>pebblenursing.com</v>
+      </c>
+      <c r="C64" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>pebblenursing.com</v>
+      </c>
+      <c r="D64" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>pinetreenursing.com</v>
+      </c>
+      <c r="C65" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>pinetreenursing.com</v>
+      </c>
+      <c r="D65" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" ref="B66:C92" si="1">A66</f>
+        <v>refugionursing.com</v>
+      </c>
+      <c r="C66" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>refugionursing.com</v>
+      </c>
+      <c r="D66" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="24" t="s">
+        <v>427</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" si="1"/>
+        <v>riverccc.com</v>
+      </c>
+      <c r="C67" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>riverccc.com</v>
+      </c>
+      <c r="D67" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="24" t="s">
+        <v>439</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>https://rockcreekhealth.com</v>
+      </c>
+      <c r="C68" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>https://rockcreekhealth.com</v>
+      </c>
+      <c r="D68" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="24" t="s">
+        <v>447</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>sansabarehab.com</v>
+      </c>
+      <c r="C69" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>sansabarehab.com</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="24" t="s">
+        <v>456</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>sevenoaksnursing.com</v>
+      </c>
+      <c r="C70" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>sevenoaksnursing.com</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="24" t="s">
+        <v>462</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>siennanursing.com</v>
+      </c>
+      <c r="C71" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>siennanursing.com</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>silvertreenursing.com</v>
+      </c>
+      <c r="C72" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>silvertreenursing.com</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="24" t="s">
+        <v>481</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>skilledcareofmexia.com</v>
+      </c>
+      <c r="C73" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>skilledcareofmexia.com</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="24" t="s">
+        <v>489</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>slatoncarecenter.com</v>
+      </c>
+      <c r="C74" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>slatoncarecenter.com</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="24" t="s">
+        <v>617</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>songbirdnursing.com</v>
+      </c>
+      <c r="C75" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>songbirdnursing.com</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>southernspecialtynursing.com</v>
+      </c>
+      <c r="C76" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>southernspecialtynursing.com</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>stgilesnursing.com</v>
+      </c>
+      <c r="C77" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>stgilesnursing.com</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="24" t="s">
+        <v>621</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>stteresanursing.com</v>
+      </c>
+      <c r="C78" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>stteresanursing.com</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>sunflowerparkhealth.com</v>
+      </c>
+      <c r="C79" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>sunflowerparkhealth.com</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="24" t="s">
+        <v>512</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>thearborsnursing.com</v>
+      </c>
+      <c r="C80" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>thearborsnursing.com</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="24" t="s">
+        <v>521</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>atriumofbellmead.com</v>
+      </c>
+      <c r="C81" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>atriumofbellmead.com</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>https://hillsnursing.com</v>
+      </c>
+      <c r="C82" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>https://hillsnursing.com</v>
+      </c>
+      <c r="D82" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>premierofalice.com</v>
+      </c>
+      <c r="C83" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>premierofalice.com</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="24" t="s">
+        <v>623</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>rioatmissiontrails.com</v>
+      </c>
+      <c r="C84" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>rioatmissiontrails.com</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="24" t="s">
+        <v>545</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>twinoakscare.com</v>
+      </c>
+      <c r="C85" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>twinoakscare.com</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>universityparknr.com</v>
+      </c>
+      <c r="C86" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>universityparknr.com</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="24" t="s">
+        <v>625</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>vidorhealth.com</v>
+      </c>
+      <c r="C87" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>vidorhealth.com</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="24" t="s">
+        <v>627</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>villatoscanarehab.com</v>
+      </c>
+      <c r="C88" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>villatoscanarehab.com</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="24" t="s">
+        <v>629</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>wellingtoncarecenter.com</v>
+      </c>
+      <c r="C89" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>wellingtoncarecenter.com</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="24" t="s">
+        <v>562</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>Westwardtrailsnursing.com/</v>
+      </c>
+      <c r="C90" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>Westwardtrailsnursing.com/</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="24" t="s">
+        <v>631</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>whisperingpinescare.com</v>
+      </c>
+      <c r="C91" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>whisperingpinescare.com</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="24" t="s">
+        <v>633</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>whisperwoodnursing.com</v>
+      </c>
+      <c r="C92" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>whisperwoodnursing.com</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="http://amarilloskilledcenter.com/" xr:uid="{BBA9B971-1A80-3140-AB89-999569F82068}"/>
+    <hyperlink ref="A2" r:id="rId2" display="http://beaumontnursingandrehab.com/" xr:uid="{F7A80318-99C0-B04D-862E-DF15E9DD4BBF}"/>
+    <hyperlink ref="A3" r:id="rId3" display="http://bertramnursing.com/" xr:uid="{4D61D2C5-A1E8-8445-9780-6AA5EA25140B}"/>
+    <hyperlink ref="A4" r:id="rId4" display="http://bigspringcenterforskilledcare.com/" xr:uid="{4C62FD13-C3E4-AE44-8F80-E4678A63A2FB}"/>
+    <hyperlink ref="A5" r:id="rId5" display="http://birchwoodnursing.com/" xr:uid="{BC3023AE-2436-5F49-BACB-844524106E48}"/>
+    <hyperlink ref="A6" r:id="rId6" display="http://bluebonnetnursing.com/" xr:uid="{B3C7623E-8110-814C-BA98-A73187682161}"/>
+    <hyperlink ref="A7" r:id="rId7" display="http://brownwoodrehab.com/" xr:uid="{222E404D-2A4B-584C-AF79-C5E44266F30A}"/>
+    <hyperlink ref="A8" r:id="rId8" display="http://buenavidanursing.com/" xr:uid="{CAA8AE1D-E2BC-2E49-BD27-E3F99E0E93C2}"/>
+    <hyperlink ref="A9" r:id="rId9" display="http://buenavidasanantonio.com/" xr:uid="{C03E4946-74F3-7F46-BA5F-946B9547E19C}"/>
+    <hyperlink ref="A10" r:id="rId10" display="http://caprocknursing.com/" xr:uid="{1F04DB70-07B5-D641-AD78-4F752BBC0BA7}"/>
+    <hyperlink ref="A11" r:id="rId11" display="http://carenursingcenter.com/" xr:uid="{14652ED4-9987-6145-8432-732EA36E5D29}"/>
+    <hyperlink ref="A12" r:id="rId12" display="http://castlepinesatlufkin.com/" xr:uid="{352660A2-1C7A-DA46-8886-B6FA34F4997A}"/>
+    <hyperlink ref="A13" r:id="rId13" display="http://cedarcreeknursing.com/" xr:uid="{D5DEE4E9-6054-964E-9971-69F74B12D992}"/>
+    <hyperlink ref="A14" r:id="rId14" display="http://centraltexasnursing.com/" xr:uid="{CA931B54-70D3-0F43-B934-4AA24DB0C1AB}"/>
+    <hyperlink ref="A15" r:id="rId15" display="http://cherokeerosenursing.com/" xr:uid="{E1846DBD-C57E-BE4A-BD0C-5A7A0E25868F}"/>
+    <hyperlink ref="A16" r:id="rId16" display="http://conchohealthandrehab.com/" xr:uid="{EC6DB312-F8FD-F847-B9A9-578740274EC1}"/>
+    <hyperlink ref="A17" r:id="rId17" display="http://cottonwoodnursing.com/" xr:uid="{1F9E93D5-6E01-CC4E-93A0-CC24218B33D0}"/>
+    <hyperlink ref="A18" r:id="rId18" display="http://countryviewnr.com/" xr:uid="{136F795D-A755-A048-93A3-3623D91BFCC3}"/>
+    <hyperlink ref="A19" r:id="rId19" display="http://crossroadsnursingandrehab.com/" xr:uid="{F00A59A0-0799-DE42-8B9D-746E8C58B588}"/>
+    <hyperlink ref="A20" r:id="rId20" display="http://deeringsnursing.com/" xr:uid="{92C59E94-0F6C-F343-8105-FFBA30A61E3D}"/>
+    <hyperlink ref="A21" r:id="rId21" display="http://deleonnursing.com/" xr:uid="{51F00958-049C-C144-9E76-53E3B300990B}"/>
+    <hyperlink ref="A22" r:id="rId22" display="http://devinehealthandrehab.com/" xr:uid="{4A7F90E3-155D-6B45-82C5-C25E68A130C7}"/>
+    <hyperlink ref="A23" r:id="rId23" display="http://dogwoodtrails.com/" xr:uid="{25E821BC-8F94-FF4B-8B8A-F093B4C6BF6D}"/>
+    <hyperlink ref="A24" r:id="rId24" display="http://eaglepassnursing.com/" xr:uid="{95CC9F36-83F8-C042-A141-56141EAE3109}"/>
+    <hyperlink ref="A25" r:id="rId25" display="http://fairfieldnursingandrehab.com/" xr:uid="{33A7E97B-51D7-5F41-9CA2-6A0C81A941E0}"/>
+    <hyperlink ref="A26" r:id="rId26" display="http://fivepointsnursing.com/" xr:uid="{1292FF37-A22D-4741-8AE2-003FD3ED693A}"/>
+    <hyperlink ref="A27" r:id="rId27" display="http://www.fivepointsdesoto.com/" xr:uid="{6ADB0B52-A01A-C24E-8B49-64F77A189043}"/>
+    <hyperlink ref="A28" r:id="rId28" display="http://fortressnursing.com/" xr:uid="{23EA6E87-AFC6-6D44-9955-052F523B951D}"/>
+    <hyperlink ref="A29" r:id="rId29" display="http://franklinheightsnursing.com/" xr:uid="{041A1DDC-0686-A949-82A0-CBC2BE829EB6}"/>
+    <hyperlink ref="A30" r:id="rId30" display="http://franklincare.com/" xr:uid="{96E73169-F90A-5641-8724-C4C8E1310EEF}"/>
+    <hyperlink ref="A31" r:id="rId31" display="http://georgiamanornursing.com/" xr:uid="{3A04AEB6-0DD7-A445-8458-85F1D24F373C}"/>
+    <hyperlink ref="A32" r:id="rId32" display="http://gilmernursing.com/" xr:uid="{35D0A689-B1EC-B246-B08C-81501C2EFDC5}"/>
+    <hyperlink ref="A34" r:id="rId33" display="http://granburycarecenter.com/" xr:uid="{8A108946-BFBF-D949-BC49-B717E8A248BC}"/>
+    <hyperlink ref="A35" r:id="rId34" display="http://greatplainsnursing.com/" xr:uid="{2033C68B-F266-4543-9DDA-5B20D807298B}"/>
+    <hyperlink ref="A36" r:id="rId35" display="http://greenbrierofpalestine.com/" xr:uid="{FD499A4C-8B30-F44A-9691-83F583F5C445}"/>
+    <hyperlink ref="A37" r:id="rId36" display="http://greenbrieroftyler.com/" xr:uid="{09D7347F-6E88-B94A-8BFF-FDA205B1D083}"/>
+    <hyperlink ref="A38" r:id="rId37" display="http://greenhillvillas.com/" xr:uid="{5B80C5E2-1C0F-BE43-BA11-D5FE05DC48CD}"/>
+    <hyperlink ref="A39" r:id="rId38" display="http://grovetonnursinghome.com/" xr:uid="{3E9937CE-D784-8B49-93C8-379D6EC13910}"/>
+    <hyperlink ref="A40" r:id="rId39" display="http://heritagehousenursing.com/" xr:uid="{3FDABFB8-07B4-0D4F-9828-743BA40A87B5}"/>
+    <hyperlink ref="A41" r:id="rId40" display="http://heritageplacedecatur.com/" xr:uid="{C9D14017-F382-C244-92B2-497ABB4B749C}"/>
+    <hyperlink ref="A42" r:id="rId41" display="http://huebnercreekhealth.com/" xr:uid="{D9DDC9C5-70E1-F54F-A399-53B38A37A93F}"/>
+    <hyperlink ref="A43" r:id="rId42" display="http://kempcarecenter.com/" xr:uid="{F3FF40DB-F6D6-C944-B876-F7055CF2858A}"/>
+    <hyperlink ref="A44" r:id="rId43" display="http://kenedyhealth.com/" xr:uid="{28FA0326-85B1-1842-B99F-95713DC5008E}"/>
+    <hyperlink ref="A45" r:id="rId44" display="http://kerenscare.com/" xr:uid="{8D957CFD-474D-4443-8669-2E4953539E58}"/>
+    <hyperlink ref="A46" r:id="rId45" display="http://labahianursing.com/" xr:uid="{5A714975-C7D6-754D-B852-4ECA4689F65B}"/>
+    <hyperlink ref="A47" r:id="rId46" display="http://lahaciendarehabcare.com/" xr:uid="{086B5864-7033-674F-8FDF-70DFD9C7B31A}"/>
+    <hyperlink ref="A48" r:id="rId47" display="http://lavidaserenanursing.com/" xr:uid="{55DE3002-A767-7E45-80CE-F8E2CC0A14AF}"/>
+    <hyperlink ref="A49" r:id="rId48" display="http://lakelodgenursing.com/" xr:uid="{520F3361-90BA-BC49-B4BB-FCF86145067B}"/>
+    <hyperlink ref="A50" r:id="rId49" display="http://lampstandnursing.com/" xr:uid="{F76E3E92-1348-724E-A60D-FE632E99E9AD}"/>
+    <hyperlink ref="A51" r:id="rId50" display="http://lubbockcarecenter.com/" xr:uid="{180864A8-53A2-9F4F-B555-2BA70E2F9293}"/>
+    <hyperlink ref="A52" r:id="rId51" display="http://madisonvillecarecenter.com/" xr:uid="{457C8BCE-D158-B640-91A1-896077AB4E50}"/>
+    <hyperlink ref="A53" r:id="rId52" display="http://marinecreeknursing.com/" xr:uid="{EDC000B2-0E84-8142-92CE-01819598C4A4}"/>
+    <hyperlink ref="A54" r:id="rId53" display="http://mcleancarecenter.com/" xr:uid="{48D85CC6-0E1C-914D-84F9-E1AB6C979B76}"/>
+    <hyperlink ref="A55" r:id="rId54" display="http://memphisconvalescent.com/" xr:uid="{31627FB7-7996-764E-89E9-FF8544EC6606}"/>
+    <hyperlink ref="A56" r:id="rId55" display="http://mesavistahealthcenter.com/" xr:uid="{4E0C995B-2DF7-1F4A-8B57-62168F0628F2}"/>
+    <hyperlink ref="A57" r:id="rId56" display="http://mineralwellsnursing.com/" xr:uid="{09982769-8B2B-374B-A291-1CD43238A9DF}"/>
+    <hyperlink ref="A58" r:id="rId57" display="http://missionridgerehab.com/" xr:uid="{1F369E44-32F2-FB43-B627-4ABA15FCC8C3}"/>
+    <hyperlink ref="A59" r:id="rId58" display="http://mountainviewnursing.com/" xr:uid="{547CB9A9-BAF0-E945-B65B-A1CB70DA064F}"/>
+    <hyperlink ref="A60" r:id="rId59" display="http://navasotanursing.com/" xr:uid="{21F12EFF-B771-3043-8451-1CEA21E746D3}"/>
+    <hyperlink ref="A61" r:id="rId60" display="http://northpointenursing.com/" xr:uid="{6F135BF0-CB6D-224A-B044-C1F4212B6EF8}"/>
+    <hyperlink ref="A62" r:id="rId61" display="http://oakridgemanornursing.com/" xr:uid="{81EC3248-CFC9-204D-B878-8BACA58259A2}"/>
+    <hyperlink ref="A63" r:id="rId62" display="http://oasisnursing.com/" xr:uid="{57581D2B-BB95-CB47-B84F-D52AD89A7061}"/>
+    <hyperlink ref="A64" r:id="rId63" display="http://pebblenursing.com/" xr:uid="{D771637C-DB9F-484E-B359-03EBB047394C}"/>
+    <hyperlink ref="A65" r:id="rId64" display="http://pinetreenursing.com/" xr:uid="{7DA0F01B-2D88-E543-B843-1714FFD3A911}"/>
+    <hyperlink ref="A66" r:id="rId65" display="http://refugionursing.com/" xr:uid="{7E131C86-E4C3-0642-99A1-D8BA02F2700F}"/>
+    <hyperlink ref="A67" r:id="rId66" display="http://riverccc.com/" xr:uid="{60893D40-6BD2-5247-9B72-DFD24406DAB0}"/>
+    <hyperlink ref="A68" r:id="rId67" display="https://rockcreekhealth.com/" xr:uid="{38397ED6-4981-C244-9EB2-6A5DA5066A87}"/>
+    <hyperlink ref="A69" r:id="rId68" display="http://sansabarehab.com/" xr:uid="{8EF37F61-67D0-BD41-A5E2-CF4B091D0E27}"/>
+    <hyperlink ref="A70" r:id="rId69" display="http://sevenoaksnursing.com/" xr:uid="{C139D8CA-7BB2-EE49-926F-1A382E944D4F}"/>
+    <hyperlink ref="A71" r:id="rId70" display="http://siennanursing.com/" xr:uid="{1A382BE7-B1FE-D34E-BAAD-20C7E5F6FEA6}"/>
+    <hyperlink ref="A72" r:id="rId71" display="http://silvertreenursing.com/" xr:uid="{EA0A9E85-0B96-1845-A433-629F0784D5D0}"/>
+    <hyperlink ref="A73" r:id="rId72" display="http://skilledcareofmexia.com/" xr:uid="{42B0FBEA-0F0F-9C4A-A501-3D7C6A1F7226}"/>
+    <hyperlink ref="A74" r:id="rId73" display="http://slatoncarecenter.com/" xr:uid="{6550E29E-75F2-BC49-B283-E20A86CFC611}"/>
+    <hyperlink ref="A75" r:id="rId74" display="http://songbirdnursing.com/" xr:uid="{762EE44E-384B-534A-A9CE-E16D5B3C44AD}"/>
+    <hyperlink ref="A76" r:id="rId75" display="http://southernspecialtynursing.com/" xr:uid="{16FE9095-4226-B24F-9A2B-E9D6E7100295}"/>
+    <hyperlink ref="A77" r:id="rId76" display="http://stgilesnursing.com/" xr:uid="{D6F9DAAA-4851-334A-AA97-8C2032685937}"/>
+    <hyperlink ref="A78" r:id="rId77" display="http://stteresanursing.com/" xr:uid="{D7ED4525-245F-5746-A50D-CB74C784B302}"/>
+    <hyperlink ref="A79" r:id="rId78" display="http://sunflowerparkhealth.com/" xr:uid="{1037B9BD-14B5-B447-8445-47149032451E}"/>
+    <hyperlink ref="A80" r:id="rId79" display="http://thearborsnursing.com/" xr:uid="{7D41D07C-35B9-7A4D-A5EF-573767CE4B42}"/>
+    <hyperlink ref="A81" r:id="rId80" display="http://atriumofbellmead.com/" xr:uid="{3A8A3EF6-B4E7-8344-BDAD-7092069E5AF6}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://hillsnursing.com/" xr:uid="{5A669DBB-3391-FD42-B482-B6CBC961C06F}"/>
+    <hyperlink ref="A83" r:id="rId82" display="http://premierofalice.com/" xr:uid="{8D5B700A-539C-D04C-96FE-654E640AAEEC}"/>
+    <hyperlink ref="A84" r:id="rId83" display="http://rioatmissiontrails.com/" xr:uid="{B733AF53-4681-114C-BB27-DED98F54C95E}"/>
+    <hyperlink ref="A85" r:id="rId84" display="http://twinoakscare.com/" xr:uid="{E897FCE6-7DB4-7246-A846-84576B8720F9}"/>
+    <hyperlink ref="A86" r:id="rId85" display="http://universityparknr.com/" xr:uid="{D9E0BEAD-CF87-C540-87F2-89DBF0081DEA}"/>
+    <hyperlink ref="A87" r:id="rId86" display="http://vidorhealth.com/" xr:uid="{4FC95220-F18E-7D4A-8C2A-6F66026A4B3B}"/>
+    <hyperlink ref="A88" r:id="rId87" display="http://villatoscanarehab.com/" xr:uid="{B28E4BBD-1C52-0B48-BD13-59F815FAFCCB}"/>
+    <hyperlink ref="A89" r:id="rId88" display="http://wellingtoncarecenter.com/" xr:uid="{203CBA8E-0015-0240-A0BF-CE5FBA45D811}"/>
+    <hyperlink ref="A90" r:id="rId89" display="http://westwardtrailsnursing.com/" xr:uid="{739E5E39-A341-474C-A34F-22B46FEB3918}"/>
+    <hyperlink ref="A91" r:id="rId90" display="http://whisperingpinescare.com/" xr:uid="{81F46453-CAF9-3841-86DF-332F12883B3E}"/>
+    <hyperlink ref="A92" r:id="rId91" display="http://whisperwoodnursing.com/" xr:uid="{54704A5A-E3BD-C347-A3A1-E6A28203EA53}"/>
+    <hyperlink ref="A33" r:id="rId92" display="http://grahamoakscare.com/" xr:uid="{16A5BD58-670E-7F49-9898-375FB63A22A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modify renameConnect script to get last menu item and change name to care portal
</commit_message>
<xml_diff>
--- a/TodoListForHeader.xlsx
+++ b/TodoListForHeader.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephlee/Projects/puppeteer-teleos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephlee/Desktop/puppeteer-teleos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E694FD-9F2B-D54D-9476-D3F70DBFFDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09496A9B-E7A8-1D49-BB69-6E7CBAE13F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26540" activeTab="3" xr2:uid="{BB39E0D0-C88E-0046-95F3-1766E0C30F43}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="23380" activeTab="3" xr2:uid="{BB39E0D0-C88E-0046-95F3-1766E0C30F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="643">
   <si>
     <t>Live 04/11/21</t>
   </si>
@@ -1975,7 +1975,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;'&quot;@&quot;'&quot;\,"/>
-    <numFmt numFmtId="170" formatCode="\'@\'\,"/>
+    <numFmt numFmtId="165" formatCode="\'@\'\,"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -2139,7 +2139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10780,8 +10780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47ABF03-C855-6B49-B3E9-76F035237A07}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C66" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10841,6 +10841,9 @@
       <c r="D3" t="s">
         <v>639</v>
       </c>
+      <c r="E3" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
@@ -10857,6 +10860,9 @@
       <c r="D4" t="s">
         <v>639</v>
       </c>
+      <c r="E4" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
@@ -10873,6 +10879,9 @@
       <c r="D5" t="s">
         <v>639</v>
       </c>
+      <c r="E5" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
@@ -10889,6 +10898,9 @@
       <c r="D6" t="s">
         <v>639</v>
       </c>
+      <c r="E6" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
@@ -10905,6 +10917,9 @@
       <c r="D7" t="s">
         <v>639</v>
       </c>
+      <c r="E7" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
@@ -10921,6 +10936,9 @@
       <c r="D8" t="s">
         <v>639</v>
       </c>
+      <c r="E8" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
@@ -10937,6 +10955,9 @@
       <c r="D9" t="s">
         <v>639</v>
       </c>
+      <c r="E9" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
@@ -10953,6 +10974,9 @@
       <c r="D10" t="s">
         <v>639</v>
       </c>
+      <c r="E10" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
@@ -10969,6 +10993,9 @@
       <c r="D11" t="s">
         <v>639</v>
       </c>
+      <c r="E11" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
@@ -10985,6 +11012,9 @@
       <c r="D12" t="s">
         <v>639</v>
       </c>
+      <c r="E12" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
@@ -11001,6 +11031,9 @@
       <c r="D13" t="s">
         <v>639</v>
       </c>
+      <c r="E13" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
@@ -11017,6 +11050,9 @@
       <c r="D14" t="s">
         <v>639</v>
       </c>
+      <c r="E14" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
@@ -11033,6 +11069,9 @@
       <c r="D15" t="s">
         <v>639</v>
       </c>
+      <c r="E15" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
@@ -11049,6 +11088,9 @@
       <c r="D16" t="s">
         <v>639</v>
       </c>
+      <c r="E16" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
@@ -11065,6 +11107,9 @@
       <c r="D17" t="s">
         <v>639</v>
       </c>
+      <c r="E17" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
@@ -11081,6 +11126,9 @@
       <c r="D18" t="s">
         <v>639</v>
       </c>
+      <c r="E18" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
@@ -11097,6 +11145,9 @@
       <c r="D19" t="s">
         <v>639</v>
       </c>
+      <c r="E19" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
@@ -11113,8 +11164,8 @@
       <c r="D20" t="s">
         <v>639</v>
       </c>
-      <c r="E20">
-        <v>1</v>
+      <c r="E20" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -11132,6 +11183,9 @@
       <c r="D21" t="s">
         <v>639</v>
       </c>
+      <c r="E21" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
@@ -11148,6 +11202,9 @@
       <c r="D22" t="s">
         <v>639</v>
       </c>
+      <c r="E22" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
@@ -11164,6 +11221,9 @@
       <c r="D23" t="s">
         <v>639</v>
       </c>
+      <c r="E23" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
@@ -11180,6 +11240,9 @@
       <c r="D24" t="s">
         <v>639</v>
       </c>
+      <c r="E24" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
@@ -11196,6 +11259,9 @@
       <c r="D25" t="s">
         <v>639</v>
       </c>
+      <c r="E25" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
@@ -11212,6 +11278,9 @@
       <c r="D26" t="s">
         <v>639</v>
       </c>
+      <c r="E26" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
@@ -11228,6 +11297,9 @@
       <c r="D27" t="s">
         <v>639</v>
       </c>
+      <c r="E27" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -11244,6 +11316,9 @@
       <c r="D28" t="s">
         <v>639</v>
       </c>
+      <c r="E28" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
@@ -11260,6 +11335,9 @@
       <c r="D29" t="s">
         <v>639</v>
       </c>
+      <c r="E29" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
@@ -11276,6 +11354,9 @@
       <c r="D30" t="s">
         <v>639</v>
       </c>
+      <c r="E30" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
@@ -11292,6 +11373,9 @@
       <c r="D31" t="s">
         <v>639</v>
       </c>
+      <c r="E31" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="24" t="s">
@@ -11308,6 +11392,9 @@
       <c r="D32" t="s">
         <v>639</v>
       </c>
+      <c r="E32" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
@@ -11324,6 +11411,9 @@
       <c r="D33" t="s">
         <v>639</v>
       </c>
+      <c r="E33" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
@@ -11340,6 +11430,9 @@
       <c r="D34" t="s">
         <v>639</v>
       </c>
+      <c r="E34" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="24" t="s">
@@ -11356,6 +11449,9 @@
       <c r="D35" t="s">
         <v>639</v>
       </c>
+      <c r="E35" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
@@ -11372,6 +11468,9 @@
       <c r="D36" t="s">
         <v>639</v>
       </c>
+      <c r="E36" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="24" t="s">
@@ -11388,6 +11487,9 @@
       <c r="D37" t="s">
         <v>639</v>
       </c>
+      <c r="E37" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -11404,8 +11506,8 @@
       <c r="D38" t="s">
         <v>639</v>
       </c>
-      <c r="E38">
-        <v>2</v>
+      <c r="E38" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -11423,6 +11525,9 @@
       <c r="D39" t="s">
         <v>639</v>
       </c>
+      <c r="E39" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="24" t="s">
@@ -11439,6 +11544,9 @@
       <c r="D40" t="s">
         <v>639</v>
       </c>
+      <c r="E40" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
@@ -11455,6 +11563,9 @@
       <c r="D41" t="s">
         <v>639</v>
       </c>
+      <c r="E41" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="24" t="s">
@@ -11471,6 +11582,9 @@
       <c r="D42" t="s">
         <v>639</v>
       </c>
+      <c r="E42" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="24" t="s">
@@ -11487,6 +11601,9 @@
       <c r="D43" t="s">
         <v>639</v>
       </c>
+      <c r="E43" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="24" t="s">
@@ -11503,6 +11620,9 @@
       <c r="D44" t="s">
         <v>639</v>
       </c>
+      <c r="E44" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="24" t="s">
@@ -11519,6 +11639,9 @@
       <c r="D45" t="s">
         <v>639</v>
       </c>
+      <c r="E45" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="24" t="s">
@@ -11535,6 +11658,9 @@
       <c r="D46" t="s">
         <v>639</v>
       </c>
+      <c r="E46" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="24" t="s">
@@ -11551,6 +11677,9 @@
       <c r="D47" t="s">
         <v>639</v>
       </c>
+      <c r="E47" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
@@ -11567,8 +11696,11 @@
       <c r="D48" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
         <v>605</v>
       </c>
@@ -11583,8 +11715,11 @@
       <c r="D49" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="24" t="s">
         <v>331</v>
       </c>
@@ -11599,8 +11734,11 @@
       <c r="D50" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="24" t="s">
         <v>339</v>
       </c>
@@ -11615,8 +11753,11 @@
       <c r="D51" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="24" t="s">
         <v>607</v>
       </c>
@@ -11631,8 +11772,11 @@
       <c r="D52" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="24" t="s">
         <v>609</v>
       </c>
@@ -11647,8 +11791,11 @@
       <c r="D53" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="24" t="s">
         <v>348</v>
       </c>
@@ -11663,8 +11810,11 @@
       <c r="D54" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="24" t="s">
         <v>358</v>
       </c>
@@ -11679,8 +11829,11 @@
       <c r="D55" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="24" t="s">
         <v>611</v>
       </c>
@@ -11695,8 +11848,11 @@
       <c r="D56" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="24" t="s">
         <v>613</v>
       </c>
@@ -11711,8 +11867,11 @@
       <c r="D57" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="24" t="s">
         <v>367</v>
       </c>
@@ -11727,8 +11886,11 @@
       <c r="D58" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="24" t="s">
         <v>374</v>
       </c>
@@ -11743,8 +11905,11 @@
       <c r="D59" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="24" t="s">
         <v>615</v>
       </c>
@@ -11759,8 +11924,11 @@
       <c r="D60" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="24" t="s">
         <v>384</v>
       </c>
@@ -11775,8 +11943,11 @@
       <c r="D61" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="24" t="s">
         <v>391</v>
       </c>
@@ -11791,8 +11962,11 @@
       <c r="D62" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="24" t="s">
         <v>398</v>
       </c>
@@ -11807,8 +11981,11 @@
       <c r="D63" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="24" t="s">
         <v>405</v>
       </c>
@@ -11823,8 +12000,11 @@
       <c r="D64" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="24" t="s">
         <v>414</v>
       </c>
@@ -11839,8 +12019,11 @@
       <c r="D65" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="24" t="s">
         <v>421</v>
       </c>
@@ -11855,8 +12038,11 @@
       <c r="D66" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
         <v>427</v>
       </c>
@@ -11871,8 +12057,11 @@
       <c r="D67" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
         <v>439</v>
       </c>
@@ -11887,8 +12076,11 @@
       <c r="D68" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="24" t="s">
         <v>447</v>
       </c>
@@ -11903,8 +12095,11 @@
       <c r="D69" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
         <v>456</v>
       </c>
@@ -11919,8 +12114,11 @@
       <c r="D70" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
         <v>462</v>
       </c>
@@ -11935,8 +12133,11 @@
       <c r="D71" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
         <v>472</v>
       </c>
@@ -11951,8 +12152,11 @@
       <c r="D72" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
         <v>481</v>
       </c>
@@ -11967,8 +12171,11 @@
       <c r="D73" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
         <v>489</v>
       </c>
@@ -11983,8 +12190,11 @@
       <c r="D74" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
         <v>617</v>
       </c>
@@ -11999,8 +12209,11 @@
       <c r="D75" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="24" t="s">
         <v>619</v>
       </c>
@@ -12015,8 +12228,11 @@
       <c r="D76" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="24" t="s">
         <v>496</v>
       </c>
@@ -12031,8 +12247,11 @@
       <c r="D77" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="24" t="s">
         <v>621</v>
       </c>
@@ -12047,8 +12266,11 @@
       <c r="D78" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
         <v>503</v>
       </c>
@@ -12063,8 +12285,11 @@
       <c r="D79" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
         <v>512</v>
       </c>
@@ -12079,8 +12304,11 @@
       <c r="D80" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
         <v>521</v>
       </c>
@@ -12095,8 +12323,11 @@
       <c r="D81" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="24" t="s">
         <v>528</v>
       </c>
@@ -12111,8 +12342,11 @@
       <c r="D82" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="24" t="s">
         <v>538</v>
       </c>
@@ -12127,8 +12361,11 @@
       <c r="D83" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="24" t="s">
         <v>623</v>
       </c>
@@ -12143,8 +12380,11 @@
       <c r="D84" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="24" t="s">
         <v>545</v>
       </c>
@@ -12159,8 +12399,11 @@
       <c r="D85" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="24" t="s">
         <v>554</v>
       </c>
@@ -12175,8 +12418,11 @@
       <c r="D86" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="24" t="s">
         <v>625</v>
       </c>
@@ -12191,8 +12437,11 @@
       <c r="D87" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="24" t="s">
         <v>627</v>
       </c>
@@ -12207,8 +12456,11 @@
       <c r="D88" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="24" t="s">
         <v>629</v>
       </c>
@@ -12223,8 +12475,11 @@
       <c r="D89" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="24" t="s">
         <v>562</v>
       </c>
@@ -12239,8 +12494,11 @@
       <c r="D90" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="24" t="s">
         <v>631</v>
       </c>
@@ -12255,8 +12513,11 @@
       <c r="D91" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="24" t="s">
         <v>633</v>
       </c>
@@ -12269,6 +12530,9 @@
         <v>whisperwoodnursing.com</v>
       </c>
       <c r="D92" t="s">
+        <v>639</v>
+      </c>
+      <c r="E92" t="s">
         <v>639</v>
       </c>
     </row>

</xml_diff>